<commit_message>
Se agrega diseño de código de barras para enviar a recaudaciones y un archivo donde se detallan errores e inconsistencias
</commit_message>
<xml_diff>
--- a/doc/Cálculo de dígito verificador.xlsx
+++ b/doc/Cálculo de dígito verificador.xlsx
@@ -1,37 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="18915" windowHeight="11820"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="18915" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>00000161920000001302843</t>
   </si>
   <si>
     <t>Dígito Verificador</t>
   </si>
+  <si>
+    <t>Suma</t>
+  </si>
+  <si>
+    <t>División</t>
+  </si>
+  <si>
+    <t>Calculo dígito verificador modulo 10</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,8 +84,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,6 +130,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -163,7 +186,7 @@
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -171,7 +194,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="7"/>
@@ -186,6 +209,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Énfasis1" xfId="4" builtinId="30"/>
@@ -199,6 +229,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -277,6 +312,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -311,6 +347,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -486,528 +523,570 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3">
         <v>15973</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="B3" s="7" t="str">
-        <f>MID(A1,LEN(A1),1)</f>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="str">
+        <f>MID(A3,LEN(A3),1)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2" t="str">
-        <f>MID($A$1,A5,1)</f>
-        <v>0</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="str">
+        <f>MID($A$3,A9,1)</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="str">
-        <f t="shared" ref="B6:B11" si="0">MID($A$1,A6,1)</f>
-        <v>0</v>
-      </c>
-      <c r="C6" t="str">
-        <f>MID($D$1,1,1)</f>
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <f>+B6*C6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1">
+      <c r="B10" s="2" t="str">
+        <f t="shared" ref="B10:B15" si="0">MID($A$3,A10,1)</f>
+        <v>0</v>
+      </c>
+      <c r="C10" t="str">
+        <f>MID($D$3,1,1)</f>
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <f>+B10*C10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>3</v>
-      </c>
-      <c r="B7" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C7" t="str">
-        <f>MID($D$1,2,1)</f>
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <f t="shared" ref="D7:D26" si="1">+B7*C7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1">
-        <v>4</v>
-      </c>
-      <c r="B8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C8" t="str">
-        <f>MID($D$1,3,1)</f>
-        <v>9</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1">
-        <v>5</v>
-      </c>
-      <c r="B9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C9" t="str">
-        <f>MID($D$1,4,1)</f>
-        <v>7</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C10" t="str">
-        <f>MID($D$1,5,1)</f>
-        <v>3</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1">
-        <v>7</v>
       </c>
       <c r="B11" s="2" t="str">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C11" t="str">
+        <f>MID($D$3,2,1)</f>
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ref="D11:D30" si="1">+B11*C11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C12" t="str">
+        <f>MID($D$3,3,1)</f>
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C13" t="str">
+        <f>MID($D$3,4,1)</f>
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>6</v>
       </c>
-      <c r="C11" t="str">
-        <f>MID($D$1,1,1)</f>
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="1"/>
+      <c r="B14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C14" t="str">
+        <f>MID($D$3,5,1)</f>
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>7</v>
+      </c>
+      <c r="B15" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1">
+      <c r="C15" t="str">
+        <f>MID($D$3,1,1)</f>
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>8</v>
       </c>
-      <c r="B12" s="4" t="str">
-        <f>MID($A$1,A12,1)</f>
-        <v>1</v>
-      </c>
-      <c r="C12" t="str">
-        <f>MID($D$1,2,1)</f>
+      <c r="B16" s="4" t="str">
+        <f>MID($A$3,A16,1)</f>
+        <v>1</v>
+      </c>
+      <c r="C16" t="str">
+        <f>MID($D$3,2,1)</f>
         <v>5</v>
       </c>
-      <c r="D12">
+      <c r="D16">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>9</v>
       </c>
-      <c r="B13" s="4" t="str">
-        <f t="shared" ref="B13:B16" si="2">MID($A$1,A13,1)</f>
+      <c r="B17" s="4" t="str">
+        <f t="shared" ref="B17:B20" si="2">MID($A$3,A17,1)</f>
         <v>9</v>
       </c>
-      <c r="C13" t="str">
-        <f>MID($D$1,3,1)</f>
+      <c r="C17" t="str">
+        <f>MID($D$3,3,1)</f>
         <v>9</v>
       </c>
-      <c r="D13">
+      <c r="D17">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>10</v>
       </c>
-      <c r="B14" s="4" t="str">
+      <c r="B18" s="4" t="str">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="C14" t="str">
-        <f>MID($D$1,4,1)</f>
+      <c r="C18" t="str">
+        <f>MID($D$3,4,1)</f>
         <v>7</v>
       </c>
-      <c r="D14">
+      <c r="D18">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="1">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>11</v>
       </c>
-      <c r="B15" s="4" t="str">
+      <c r="B19" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="C15" t="str">
-        <f>MID($D$1,5,1)</f>
+      <c r="C19" t="str">
+        <f>MID($D$3,5,1)</f>
         <v>3</v>
       </c>
-      <c r="D15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="1">
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>12</v>
       </c>
-      <c r="B16" s="4" t="str">
+      <c r="B20" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="C16" t="str">
-        <f>MID($D$1,1,1)</f>
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1">
+      <c r="C20" t="str">
+        <f>MID($D$3,1,1)</f>
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>13</v>
       </c>
-      <c r="B17" s="5" t="str">
-        <f>MID($A$1,A17,1)</f>
-        <v>0</v>
-      </c>
-      <c r="C17" t="str">
-        <f>MID($D$1,2,1)</f>
+      <c r="B21" s="5" t="str">
+        <f>MID($A$3,A21,1)</f>
+        <v>0</v>
+      </c>
+      <c r="C21" t="str">
+        <f>MID($D$3,2,1)</f>
         <v>5</v>
       </c>
-      <c r="D17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1">
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>14</v>
       </c>
-      <c r="B18" s="5" t="str">
-        <f t="shared" ref="B18:B26" si="3">MID($A$1,A18,1)</f>
-        <v>0</v>
-      </c>
-      <c r="C18" t="str">
-        <f>MID($D$1,3,1)</f>
+      <c r="B22" s="5" t="str">
+        <f t="shared" ref="B22:B30" si="3">MID($A$3,A22,1)</f>
+        <v>0</v>
+      </c>
+      <c r="C22" t="str">
+        <f>MID($D$3,3,1)</f>
         <v>9</v>
       </c>
-      <c r="D18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1">
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>15</v>
       </c>
-      <c r="B19" s="5" t="str">
+      <c r="B23" s="5" t="str">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="C19" t="str">
-        <f>MID($D$1,4,1)</f>
+      <c r="C23" t="str">
+        <f>MID($D$3,4,1)</f>
         <v>7</v>
       </c>
-      <c r="D19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1">
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>16</v>
       </c>
-      <c r="B20" s="5" t="str">
+      <c r="B24" s="5" t="str">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="C20" t="str">
-        <f>MID($D$1,5,1)</f>
+      <c r="C24" t="str">
+        <f>MID($D$3,5,1)</f>
         <v>3</v>
       </c>
-      <c r="D20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1">
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>17</v>
       </c>
-      <c r="B21" s="5" t="str">
+      <c r="B25" s="5" t="str">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="C21" t="str">
-        <f>MID($D$1,1,1)</f>
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1">
+      <c r="C25" t="str">
+        <f>MID($D$3,1,1)</f>
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>18</v>
       </c>
-      <c r="B22" s="5" t="str">
+      <c r="B26" s="5" t="str">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="C22" t="str">
-        <f>MID($D$1,2,1)</f>
+      <c r="C26" t="str">
+        <f>MID($D$3,2,1)</f>
         <v>5</v>
       </c>
-      <c r="D22">
+      <c r="D26">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="1">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>19</v>
       </c>
-      <c r="B23" s="5" t="str">
+      <c r="B27" s="5" t="str">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="C23" t="str">
-        <f>MID($D$1,3,1)</f>
+      <c r="C27" t="str">
+        <f>MID($D$3,3,1)</f>
         <v>9</v>
       </c>
-      <c r="D23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="1">
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>20</v>
       </c>
-      <c r="B24" s="5" t="str">
+      <c r="B28" s="5" t="str">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="C24" t="str">
-        <f>MID($D$1,4,1)</f>
+      <c r="C28" t="str">
+        <f>MID($D$3,4,1)</f>
         <v>7</v>
       </c>
-      <c r="D24">
+      <c r="D28">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="1">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>21</v>
       </c>
-      <c r="B25" s="5" t="str">
+      <c r="B29" s="5" t="str">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="C25" t="str">
-        <f>MID($D$1,5,1)</f>
+      <c r="C29" t="str">
+        <f>MID($D$3,5,1)</f>
         <v>3</v>
       </c>
-      <c r="D25">
+      <c r="D29">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="1">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>22</v>
       </c>
-      <c r="B26" s="5" t="str">
+      <c r="B30" s="5" t="str">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="C26" t="str">
-        <f>MID($D$1,1,1)</f>
-        <v>1</v>
-      </c>
-      <c r="D26">
+      <c r="C30" t="str">
+        <f>MID($D$3,1,1)</f>
+        <v>1</v>
+      </c>
+      <c r="D30">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="1">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>23</v>
       </c>
-      <c r="B27" t="str">
-        <f>MID($E$22,A27,1)</f>
+      <c r="B31" t="str">
+        <f t="shared" ref="B31:B39" si="4">MID($E$26,A31,1)</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="1">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>24</v>
       </c>
-      <c r="B28" t="str">
-        <f>MID($E$22,A28,1)</f>
+      <c r="B32" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="1">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>25</v>
       </c>
-      <c r="B29" t="str">
-        <f>MID($E$22,A29,1)</f>
+      <c r="B33" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="1">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>26</v>
       </c>
-      <c r="B30" t="str">
-        <f>MID($E$22,A30,1)</f>
+      <c r="B34" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="1">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
         <v>27</v>
       </c>
-      <c r="B31" t="str">
-        <f>MID($E$22,A31,1)</f>
+      <c r="B35" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="1">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>28</v>
       </c>
-      <c r="B32" t="str">
-        <f>MID($E$22,A32,1)</f>
+      <c r="B36" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="1">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>29</v>
       </c>
-      <c r="B33" t="str">
-        <f>MID($E$22,A33,1)</f>
+      <c r="B37" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A34" s="1">
+    <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
         <v>30</v>
       </c>
-      <c r="B34" t="str">
-        <f>MID($E$22,A34,1)</f>
+      <c r="B38" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="1">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
         <v>31</v>
       </c>
-      <c r="B35" t="str">
-        <f>MID($E$22,A35,1)</f>
+      <c r="B39" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="F35" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="20.25" thickBot="1">
-      <c r="D36">
-        <f>SUM(D6:D35)</f>
+      <c r="D39" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D40">
+        <f>SUM(D10:D39)</f>
         <v>167</v>
       </c>
-      <c r="E36">
-        <f>INT(D36/2)</f>
+      <c r="E40">
+        <f>INT(D40/2)</f>
         <v>83</v>
       </c>
-      <c r="F36" s="9">
-        <f>MOD(E36,10)</f>
+      <c r="F40" s="9">
+        <f>MOD(E40,10)</f>
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>